<commit_message>
Updated ER model and added SQL password to gitignore
</commit_message>
<xml_diff>
--- a/ER_model.xlsx
+++ b/ER_model.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/1st Year Msc/2nd Semester/COMP30830 - Software Engineering/Assignments/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{7ABC74DD-58FD-482F-A121-BC2FFA856E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E9C7E8C-AA9B-477B-A2E9-15872339B465}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="8_{7ABC74DD-58FD-482F-A121-BC2FFA856E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B738C92F-D7A1-46F1-A996-A0EE73AF4768}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{73237B70-3A82-4ECA-8AFA-B82A64E8A930}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73237B70-3A82-4ECA-8AFA-B82A64E8A930}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="ER Diagram" sheetId="2" r:id="rId2"/>
+    <sheet name="ER Diagram" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,77 +33,6 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
-  <si>
-    <t>Realtime</t>
-  </si>
-  <si>
-    <t>Station Number</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Bike availability</t>
-  </si>
-  <si>
-    <t>Parking availability</t>
-  </si>
-  <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
-    <t>Pearse Street</t>
-  </si>
-  <si>
-    <t>Day</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Real time</t>
-  </si>
-  <si>
-    <t>Forecast</t>
-  </si>
-  <si>
-    <t>Temperature</t>
-  </si>
-  <si>
-    <t>Precipitation</t>
-  </si>
-  <si>
-    <t>Hour</t>
-  </si>
-  <si>
-    <t>1st API call</t>
-  </si>
-  <si>
-    <t>2nd API call</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
@@ -116,18 +44,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -148,12 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -183,8 +102,8 @@
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>31750</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -199,8 +118,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4349750" y="139700"/>
-          <a:ext cx="1778000" cy="1543050"/>
+          <a:off x="4149725" y="139700"/>
+          <a:ext cx="1692275" cy="1860550"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -236,14 +155,14 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-IE" sz="1600"/>
-            <a:t>Number (PK)</a:t>
+            <a:t>Name (PK)</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-IE" sz="1600"/>
-            <a:t>Name</a:t>
+            <a:t>Address</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -259,6 +178,13 @@
           <a:r>
             <a:rPr lang="en-IE" sz="1600" baseline="0"/>
             <a:t>Latitude</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Bike Stands</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -281,10 +207,10 @@
       <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -299,8 +225,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7499350" y="196850"/>
-          <a:ext cx="1778000" cy="1543050"/>
+          <a:off x="7156450" y="203200"/>
+          <a:ext cx="2797175" cy="2597150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -344,7 +270,42 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-IE" sz="1600" baseline="0"/>
-            <a:t>Time (PK)</a:t>
+            <a:t>Weekday_or_weekend</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Day</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Month</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Year</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Bikes_Available</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>Spaces_Available</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -353,6 +314,62 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>168275</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0125BA14-BB7B-4EB6-9B68-A0BF2A5260FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="2" idx="3"/>
+          <a:endCxn id="3" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5842000" y="1069975"/>
+          <a:ext cx="1314450" cy="431800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -654,276 +671,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BEF948C-46BA-4649-8894-F39FBC10C2C4}">
-  <dimension ref="A1:M16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
-        <v>7</v>
-      </c>
-      <c r="L2" t="s">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>2022</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
-      </c>
-      <c r="J3">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.41805555555555557</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-      <c r="D5">
-        <v>2022</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E7" s="2"/>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" t="s">
-        <v>3</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E11" s="1">
-        <v>44843</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11" s="1">
-        <v>44602</v>
-      </c>
-      <c r="J11">
-        <v>7</v>
-      </c>
-      <c r="K11">
-        <v>11</v>
-      </c>
-      <c r="L11">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12" s="1">
-        <v>44602</v>
-      </c>
-      <c r="J12">
-        <v>8</v>
-      </c>
-      <c r="K12">
-        <v>12</v>
-      </c>
-      <c r="L12">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="E14" s="1">
-        <v>44602</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14" s="1">
-        <v>44602</v>
-      </c>
-      <c r="J14">
-        <v>7</v>
-      </c>
-      <c r="K14">
-        <v>12</v>
-      </c>
-      <c r="L14">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>44602</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-      <c r="E16">
-        <v>12</v>
-      </c>
-      <c r="F16">
-        <v>40</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCDC8A7-AEE6-4780-A70C-F0F3053C82EC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="8.7265625" style="4"/>
+    <col min="1" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated ER diagram with weather data
</commit_message>
<xml_diff>
--- a/ER_model.xlsx
+++ b/ER_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/1st Year Msc/2nd Semester/COMP30830 - Software Engineering/Assignments/Group_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="8_{7ABC74DD-58FD-482F-A121-BC2FFA856E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B738C92F-D7A1-46F1-A996-A0EE73AF4768}"/>
+  <xr:revisionPtr revIDLastSave="161" documentId="8_{7ABC74DD-58FD-482F-A121-BC2FFA856E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD37295B-E2BE-4AFA-8684-844DB5271E55}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{73237B70-3A82-4ECA-8AFA-B82A64E8A930}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{73237B70-3A82-4ECA-8AFA-B82A64E8A930}"/>
   </bookViews>
   <sheets>
     <sheet name="ER Diagram" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,44 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+  <si>
+    <t>In_x_seconds</t>
+  </si>
+  <si>
+    <t>in 1 minute</t>
+  </si>
+  <si>
+    <t>in 2 minutes</t>
+  </si>
+  <si>
+    <t>in 7 days</t>
+  </si>
+  <si>
+    <t>New data</t>
+  </si>
+  <si>
+    <t>Time now</t>
+  </si>
+  <si>
+    <t>In_x_second</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>API call @ 11:30</t>
+  </si>
+  <si>
+    <t>API call @ 11:31</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -70,9 +108,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -370,6 +409,308 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>507999</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rectangle 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15BA622B-8FE5-4AF1-8BA6-993EEBF6C692}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="752474" y="920750"/>
+          <a:ext cx="2803525" cy="3790950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="2000"/>
+            <a:t>Weather_realtime</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>dt (PK) - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>sunrise - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>sunset - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>temp - int (convert to celcius)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>feels_like - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>pressure - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>humidity - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>clouds - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>visibility - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>main - VARCHAR(100)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>description - VARCHAR(100)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>icon - VARCHAR(6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-IE" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>415924</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30F7E1C7-9B67-4DEC-A6E8-61D0034BA1AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4073524" y="2590800"/>
+          <a:ext cx="2803525" cy="3790950"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="2000"/>
+            <a:t>Weather_forecast</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>dt (PK) - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>sunrise - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>sunset - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>temp - int (convert to celcius)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>feels_like - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>pressure - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>humidity - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>clouds - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>visibility - int</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>main - VARCHAR(100)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>description - VARCHAR(100)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-IE" sz="1600" baseline="0"/>
+            <a:t>icon - VARCHAR(6)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-IE" sz="2000"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -672,17 +1013,212 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCDC8A7-AEE6-4780-A70C-F0F3053C82EC}">
-  <dimension ref="A1"/>
+  <dimension ref="M17:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.7109375" style="1"/>
+    <col min="1" max="12" width="8.7265625" style="1"/>
+    <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.7265625" style="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="17" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0</v>
+      </c>
+      <c r="P17" s="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="N18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q18" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" s="1">
+        <v>60</v>
+      </c>
+      <c r="P19" s="1">
+        <v>120</v>
+      </c>
+      <c r="Q19" s="1">
+        <f>P19-P17</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N20" s="1">
+        <v>120</v>
+      </c>
+      <c r="P20" s="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N21" s="1">
+        <v>11111111</v>
+      </c>
+    </row>
+    <row r="24" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="N24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M25" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M26" s="2">
+        <v>0.47986111111111113</v>
+      </c>
+      <c r="N26" s="1">
+        <v>60</v>
+      </c>
+      <c r="O26" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M27" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="N27" s="1">
+        <v>120</v>
+      </c>
+      <c r="O27" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M28" s="2">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="N28" s="1">
+        <v>180</v>
+      </c>
+      <c r="O28" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="29" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="M29" s="2">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="N29" s="1">
+        <v>240</v>
+      </c>
+      <c r="O29" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="N31" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="13:17" x14ac:dyDescent="0.35">
+      <c r="N32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M33" s="2">
+        <v>0.48055555555555557</v>
+      </c>
+      <c r="N33" s="1">
+        <v>120</v>
+      </c>
+      <c r="O33" s="1">
+        <f>N33-60</f>
+        <v>60</v>
+      </c>
+      <c r="P33" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M34" s="2">
+        <v>0.48125000000000001</v>
+      </c>
+      <c r="N34" s="1">
+        <v>180</v>
+      </c>
+      <c r="O34" s="1">
+        <f t="shared" ref="O34:O36" si="0">N34-60</f>
+        <v>120</v>
+      </c>
+      <c r="P34" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="35" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M35" s="2">
+        <v>0.48194444444444445</v>
+      </c>
+      <c r="N35" s="1">
+        <v>240</v>
+      </c>
+      <c r="O35" s="1">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
+      <c r="P35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="13:16" x14ac:dyDescent="0.35">
+      <c r="M36" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="N36" s="1">
+        <v>300</v>
+      </c>
+      <c r="O36" s="1">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+      <c r="P36" s="1">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Creates weather forecast table
</commit_message>
<xml_diff>
--- a/ER_model.xlsx
+++ b/ER_model.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucd-my.sharepoint.com/personal/michael_davitt_ucdconnect_ie/Documents/Documents/1st Year Msc/2nd Semester/COMP30830 - Software Engineering/Assignments/Group_Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tarik\Desktop\UCD Works\SoftwareEngeneering\COMP30830_COVID_Bikes_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="161" documentId="8_{7ABC74DD-58FD-482F-A121-BC2FFA856E41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD37295B-E2BE-4AFA-8684-844DB5271E55}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{73237B70-3A82-4ECA-8AFA-B82A64E8A930}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="ER Diagram" sheetId="2" r:id="rId1"/>
@@ -72,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -625,7 +624,7 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-IE" sz="1600" baseline="0"/>
-            <a:t>dt (PK) - int</a:t>
+            <a:t>dt (PK) - VARCHAR(100)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -1012,21 +1011,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CCDC8A7-AEE6-4780-A70C-F0F3053C82EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="M17:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
       <selection activeCell="Q31" sqref="Q31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="12" width="8.7265625" style="1"/>
+    <col min="1" max="12" width="8.7109375" style="1"/>
     <col min="13" max="13" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="1"/>
+    <col min="14" max="16384" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M17" s="1" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1036,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N18" s="1" t="s">
         <v>0</v>
       </c>
@@ -1048,7 +1047,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M19" s="1" t="s">
         <v>1</v>
       </c>
@@ -1063,7 +1062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="20" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M20" s="1" t="s">
         <v>2</v>
       </c>
@@ -1074,7 +1073,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="21" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M21" s="1" t="s">
         <v>3</v>
       </c>
@@ -1082,12 +1081,12 @@
         <v>11111111</v>
       </c>
     </row>
-    <row r="24" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="24" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="25" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M25" s="2">
         <v>0.47916666666666669</v>
       </c>
@@ -1098,7 +1097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="26" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M26" s="2">
         <v>0.47986111111111113</v>
       </c>
@@ -1109,7 +1108,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="27" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M27" s="2">
         <v>0.48055555555555557</v>
       </c>
@@ -1120,7 +1119,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="28" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M28" s="2">
         <v>0.48125000000000001</v>
       </c>
@@ -1131,7 +1130,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="29" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="29" spans="13:17" x14ac:dyDescent="0.25">
       <c r="M29" s="2">
         <v>0.48194444444444445</v>
       </c>
@@ -1142,12 +1141,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="31" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N31" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="13:17" x14ac:dyDescent="0.35">
+    <row r="32" spans="13:17" x14ac:dyDescent="0.25">
       <c r="N32" s="1" t="s">
         <v>7</v>
       </c>
@@ -1158,7 +1157,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="33" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M33" s="2">
         <v>0.48055555555555557</v>
       </c>
@@ -1173,7 +1172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="34" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M34" s="2">
         <v>0.48125000000000001</v>
       </c>
@@ -1188,7 +1187,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="35" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="35" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M35" s="2">
         <v>0.48194444444444445</v>
       </c>
@@ -1203,7 +1202,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="13:16" x14ac:dyDescent="0.35">
+    <row r="36" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M36" s="2">
         <v>0.4826388888888889</v>
       </c>

</xml_diff>